<commit_message>
Export project data to Excel
</commit_message>
<xml_diff>
--- a/project-data.xlsx
+++ b/project-data.xlsx
@@ -919,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
   </sheetData>
@@ -1168,10 +1168,10 @@
         <v>48</v>
       </c>
       <c r="R2" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S2" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1227,10 +1227,10 @@
         <v>55</v>
       </c>
       <c r="R3" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S3" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1286,10 +1286,10 @@
         <v>65</v>
       </c>
       <c r="R4" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S4" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1345,10 +1345,10 @@
         <v>73</v>
       </c>
       <c r="R5" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S5" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1404,10 +1404,10 @@
         <v>79</v>
       </c>
       <c r="R6" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S6" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1463,10 +1463,10 @@
         <v>88</v>
       </c>
       <c r="R7" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S7" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1522,10 +1522,10 @@
         <v>92</v>
       </c>
       <c r="R8" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S8" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1581,10 +1581,10 @@
         <v>100</v>
       </c>
       <c r="R9" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S9" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1640,10 +1640,10 @@
         <v>107</v>
       </c>
       <c r="R10" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S10" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1699,10 +1699,10 @@
         <v>114</v>
       </c>
       <c r="R11" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
       <c r="S11" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
   </sheetData>
@@ -1770,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1862,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
   </sheetData>
@@ -1935,7 +1935,7 @@
         <v>137</v>
       </c>
       <c r="H2" s="2">
-        <v>45924.65339482639</v>
+        <v>45924.934645208334</v>
       </c>
     </row>
   </sheetData>
@@ -1988,7 +1988,7 @@
         <v>142</v>
       </c>
       <c r="E2" s="2">
-        <v>45924.570061493054</v>
+        <v>45924.851311875</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2005,7 +2005,7 @@
         <v>145</v>
       </c>
       <c r="E3" s="2">
-        <v>45923.65339482639</v>
+        <v>45923.934645208334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>